<commit_message>
Finished initial leg work so that i can tweak the model and explore its capabilities qualitatively
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -33889,125 +33889,125 @@
   </sheetData>
   <mergeCells count="120">
     <mergeCell ref="A2:A56"/>
+    <mergeCell ref="A387:A441"/>
+    <mergeCell ref="A772:A826"/>
+    <mergeCell ref="A167:A221"/>
+    <mergeCell ref="A552:A606"/>
+    <mergeCell ref="A937:A991"/>
+    <mergeCell ref="A332:A386"/>
+    <mergeCell ref="A717:A771"/>
+    <mergeCell ref="A112:A166"/>
+    <mergeCell ref="A497:A551"/>
+    <mergeCell ref="A882:A936"/>
+    <mergeCell ref="A277:A331"/>
+    <mergeCell ref="A662:A716"/>
+    <mergeCell ref="A1047:A1101"/>
     <mergeCell ref="A57:A111"/>
-    <mergeCell ref="A112:A166"/>
-    <mergeCell ref="A167:A221"/>
+    <mergeCell ref="A442:A496"/>
+    <mergeCell ref="A827:A881"/>
     <mergeCell ref="A222:A276"/>
-    <mergeCell ref="A277:A331"/>
-    <mergeCell ref="A332:A386"/>
-    <mergeCell ref="A387:A441"/>
-    <mergeCell ref="A442:A496"/>
-    <mergeCell ref="A497:A551"/>
-    <mergeCell ref="A552:A606"/>
     <mergeCell ref="A607:A661"/>
-    <mergeCell ref="A662:A716"/>
-    <mergeCell ref="A717:A771"/>
-    <mergeCell ref="A772:A826"/>
-    <mergeCell ref="A827:A881"/>
-    <mergeCell ref="A882:A936"/>
-    <mergeCell ref="A937:A991"/>
     <mergeCell ref="A992:A1046"/>
-    <mergeCell ref="A1047:A1101"/>
     <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B519:B529"/>
+    <mergeCell ref="B1036:B1046"/>
     <mergeCell ref="B13:B23"/>
+    <mergeCell ref="B530:B540"/>
+    <mergeCell ref="B1047:B1057"/>
     <mergeCell ref="B24:B34"/>
+    <mergeCell ref="B541:B551"/>
+    <mergeCell ref="B1058:B1068"/>
     <mergeCell ref="B35:B45"/>
+    <mergeCell ref="B552:B562"/>
+    <mergeCell ref="B1069:B1079"/>
     <mergeCell ref="B46:B56"/>
+    <mergeCell ref="B563:B573"/>
+    <mergeCell ref="B1080:B1090"/>
     <mergeCell ref="B57:B67"/>
+    <mergeCell ref="B574:B584"/>
+    <mergeCell ref="B1091:B1101"/>
     <mergeCell ref="B68:B78"/>
+    <mergeCell ref="B585:B595"/>
     <mergeCell ref="B79:B89"/>
+    <mergeCell ref="B596:B606"/>
     <mergeCell ref="B90:B100"/>
+    <mergeCell ref="B607:B617"/>
     <mergeCell ref="B101:B111"/>
+    <mergeCell ref="B618:B628"/>
     <mergeCell ref="B112:B122"/>
+    <mergeCell ref="B629:B639"/>
     <mergeCell ref="B123:B133"/>
+    <mergeCell ref="B640:B650"/>
     <mergeCell ref="B134:B144"/>
+    <mergeCell ref="B651:B661"/>
     <mergeCell ref="B145:B155"/>
+    <mergeCell ref="B662:B672"/>
     <mergeCell ref="B156:B166"/>
+    <mergeCell ref="B673:B683"/>
     <mergeCell ref="B167:B177"/>
+    <mergeCell ref="B684:B694"/>
     <mergeCell ref="B178:B188"/>
+    <mergeCell ref="B695:B705"/>
     <mergeCell ref="B189:B199"/>
+    <mergeCell ref="B706:B716"/>
     <mergeCell ref="B200:B210"/>
+    <mergeCell ref="B717:B727"/>
     <mergeCell ref="B211:B221"/>
+    <mergeCell ref="B728:B738"/>
     <mergeCell ref="B222:B232"/>
+    <mergeCell ref="B739:B749"/>
     <mergeCell ref="B233:B243"/>
+    <mergeCell ref="B750:B760"/>
     <mergeCell ref="B244:B254"/>
+    <mergeCell ref="B761:B771"/>
     <mergeCell ref="B255:B265"/>
+    <mergeCell ref="B772:B782"/>
     <mergeCell ref="B266:B276"/>
+    <mergeCell ref="B783:B793"/>
     <mergeCell ref="B277:B287"/>
+    <mergeCell ref="B794:B804"/>
     <mergeCell ref="B288:B298"/>
+    <mergeCell ref="B805:B815"/>
     <mergeCell ref="B299:B309"/>
+    <mergeCell ref="B816:B826"/>
     <mergeCell ref="B310:B320"/>
+    <mergeCell ref="B827:B837"/>
     <mergeCell ref="B321:B331"/>
+    <mergeCell ref="B838:B848"/>
     <mergeCell ref="B332:B342"/>
+    <mergeCell ref="B849:B859"/>
     <mergeCell ref="B343:B353"/>
+    <mergeCell ref="B860:B870"/>
     <mergeCell ref="B354:B364"/>
+    <mergeCell ref="B871:B881"/>
     <mergeCell ref="B365:B375"/>
+    <mergeCell ref="B882:B892"/>
     <mergeCell ref="B376:B386"/>
+    <mergeCell ref="B893:B903"/>
     <mergeCell ref="B387:B397"/>
+    <mergeCell ref="B904:B914"/>
     <mergeCell ref="B398:B408"/>
+    <mergeCell ref="B915:B925"/>
     <mergeCell ref="B409:B419"/>
+    <mergeCell ref="B926:B936"/>
     <mergeCell ref="B420:B430"/>
+    <mergeCell ref="B937:B947"/>
     <mergeCell ref="B431:B441"/>
+    <mergeCell ref="B948:B958"/>
     <mergeCell ref="B442:B452"/>
+    <mergeCell ref="B959:B969"/>
     <mergeCell ref="B453:B463"/>
+    <mergeCell ref="B970:B980"/>
     <mergeCell ref="B464:B474"/>
+    <mergeCell ref="B981:B991"/>
     <mergeCell ref="B475:B485"/>
+    <mergeCell ref="B992:B1002"/>
     <mergeCell ref="B486:B496"/>
+    <mergeCell ref="B1003:B1013"/>
     <mergeCell ref="B497:B507"/>
+    <mergeCell ref="B1014:B1024"/>
     <mergeCell ref="B508:B518"/>
-    <mergeCell ref="B519:B529"/>
-    <mergeCell ref="B530:B540"/>
-    <mergeCell ref="B541:B551"/>
-    <mergeCell ref="B552:B562"/>
-    <mergeCell ref="B563:B573"/>
-    <mergeCell ref="B574:B584"/>
-    <mergeCell ref="B585:B595"/>
-    <mergeCell ref="B596:B606"/>
-    <mergeCell ref="B607:B617"/>
-    <mergeCell ref="B618:B628"/>
-    <mergeCell ref="B629:B639"/>
-    <mergeCell ref="B640:B650"/>
-    <mergeCell ref="B651:B661"/>
-    <mergeCell ref="B662:B672"/>
-    <mergeCell ref="B673:B683"/>
-    <mergeCell ref="B684:B694"/>
-    <mergeCell ref="B695:B705"/>
-    <mergeCell ref="B706:B716"/>
-    <mergeCell ref="B717:B727"/>
-    <mergeCell ref="B728:B738"/>
-    <mergeCell ref="B739:B749"/>
-    <mergeCell ref="B750:B760"/>
-    <mergeCell ref="B761:B771"/>
-    <mergeCell ref="B772:B782"/>
-    <mergeCell ref="B783:B793"/>
-    <mergeCell ref="B794:B804"/>
-    <mergeCell ref="B805:B815"/>
-    <mergeCell ref="B816:B826"/>
-    <mergeCell ref="B827:B837"/>
-    <mergeCell ref="B838:B848"/>
-    <mergeCell ref="B849:B859"/>
-    <mergeCell ref="B860:B870"/>
-    <mergeCell ref="B871:B881"/>
-    <mergeCell ref="B882:B892"/>
-    <mergeCell ref="B893:B903"/>
-    <mergeCell ref="B904:B914"/>
-    <mergeCell ref="B915:B925"/>
-    <mergeCell ref="B926:B936"/>
-    <mergeCell ref="B937:B947"/>
-    <mergeCell ref="B948:B958"/>
-    <mergeCell ref="B959:B969"/>
-    <mergeCell ref="B970:B980"/>
-    <mergeCell ref="B981:B991"/>
-    <mergeCell ref="B992:B1002"/>
-    <mergeCell ref="B1003:B1013"/>
-    <mergeCell ref="B1014:B1024"/>
     <mergeCell ref="B1025:B1035"/>
-    <mergeCell ref="B1036:B1046"/>
-    <mergeCell ref="B1047:B1057"/>
-    <mergeCell ref="B1058:B1068"/>
-    <mergeCell ref="B1069:B1079"/>
-    <mergeCell ref="B1080:B1090"/>
-    <mergeCell ref="B1091:B1101"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>